<commit_message>
update XLBH anh TuanBG
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang8/2.XulyBH/XLBH2208_TienLong.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang8/2.XulyBH/XLBH2208_TienLong.xlsx
@@ -640,6 +640,30 @@
     <xf numFmtId="1" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -655,32 +679,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -992,7 +992,7 @@
   <dimension ref="A1:X115"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1024,43 +1024,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="73" t="s">
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="73"/>
+      <c r="F2" s="65"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -1105,58 +1105,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="69" t="s">
+      <c r="A4" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69" t="s">
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="69" t="s">
+      <c r="K4" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="69"/>
-      <c r="M4" s="66" t="s">
+      <c r="L4" s="61"/>
+      <c r="M4" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="66" t="s">
+      <c r="N4" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="66" t="s">
+      <c r="O4" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="64" t="s">
+      <c r="P4" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="66" t="s">
+      <c r="Q4" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="66" t="s">
+      <c r="R4" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="68" t="s">
+      <c r="S4" s="74" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="69" t="s">
+      <c r="U4" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="69" t="s">
+      <c r="V4" s="61" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="74"/>
+      <c r="A5" s="66"/>
       <c r="B5" s="57" t="s">
         <v>1</v>
       </c>
@@ -1181,23 +1181,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="69"/>
+      <c r="J5" s="61"/>
       <c r="K5" s="57" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="67"/>
-      <c r="N5" s="67"/>
-      <c r="O5" s="67"/>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="67"/>
-      <c r="S5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="68"/>
+      <c r="P5" s="73"/>
+      <c r="Q5" s="68"/>
+      <c r="R5" s="68"/>
+      <c r="S5" s="74"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="69"/>
-      <c r="V5" s="69"/>
+      <c r="U5" s="61"/>
+      <c r="V5" s="61"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1249,7 +1249,7 @@
       <c r="R6" s="2"/>
       <c r="S6" s="3"/>
       <c r="T6" s="56"/>
-      <c r="U6" s="61" t="s">
+      <c r="U6" s="69" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -1280,7 +1280,7 @@
       <c r="R7" s="2"/>
       <c r="S7" s="3"/>
       <c r="T7" s="56"/>
-      <c r="U7" s="62"/>
+      <c r="U7" s="70"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -1309,7 +1309,7 @@
       <c r="R8" s="2"/>
       <c r="S8" s="3"/>
       <c r="T8" s="56"/>
-      <c r="U8" s="62"/>
+      <c r="U8" s="70"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1338,7 +1338,7 @@
       <c r="R9" s="2"/>
       <c r="S9" s="3"/>
       <c r="T9" s="56"/>
-      <c r="U9" s="62"/>
+      <c r="U9" s="70"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -1367,7 +1367,7 @@
       <c r="R10" s="2"/>
       <c r="S10" s="3"/>
       <c r="T10" s="56"/>
-      <c r="U10" s="62"/>
+      <c r="U10" s="70"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -1396,7 +1396,7 @@
       <c r="R11" s="2"/>
       <c r="S11" s="3"/>
       <c r="T11" s="56"/>
-      <c r="U11" s="62"/>
+      <c r="U11" s="70"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -1425,7 +1425,7 @@
       <c r="R12" s="2"/>
       <c r="S12" s="3"/>
       <c r="T12" s="56"/>
-      <c r="U12" s="61" t="s">
+      <c r="U12" s="69" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -1456,7 +1456,7 @@
       <c r="R13" s="2"/>
       <c r="S13" s="3"/>
       <c r="T13" s="56"/>
-      <c r="U13" s="62"/>
+      <c r="U13" s="70"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -1485,7 +1485,7 @@
       <c r="R14" s="2"/>
       <c r="S14" s="3"/>
       <c r="T14" s="56"/>
-      <c r="U14" s="62"/>
+      <c r="U14" s="70"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -1514,7 +1514,7 @@
       <c r="R15" s="2"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="62"/>
+      <c r="U15" s="70"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -1543,7 +1543,7 @@
       <c r="R16" s="2"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="63"/>
+      <c r="U16" s="71"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -3259,6 +3259,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -3270,13 +3277,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3320,43 +3320,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="73" t="s">
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="73"/>
+      <c r="F2" s="65"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
@@ -3401,58 +3401,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="69" t="s">
+      <c r="A4" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69" t="s">
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="69" t="s">
+      <c r="K4" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="69"/>
-      <c r="M4" s="66" t="s">
+      <c r="L4" s="61"/>
+      <c r="M4" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="66" t="s">
+      <c r="N4" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="69" t="s">
+      <c r="O4" s="61" t="s">
         <v>7</v>
       </c>
       <c r="P4" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="69" t="s">
+      <c r="Q4" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="69" t="s">
+      <c r="R4" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="68" t="s">
+      <c r="S4" s="74" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="69" t="s">
+      <c r="U4" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="69" t="s">
+      <c r="V4" s="61" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="74"/>
+      <c r="A5" s="66"/>
       <c r="B5" s="41" t="s">
         <v>1</v>
       </c>
@@ -3477,23 +3477,23 @@
       <c r="I5" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="69"/>
+      <c r="J5" s="61"/>
       <c r="K5" s="41" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="67"/>
-      <c r="N5" s="67"/>
-      <c r="O5" s="69"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="61"/>
       <c r="P5" s="75"/>
-      <c r="Q5" s="69"/>
-      <c r="R5" s="69"/>
-      <c r="S5" s="68"/>
+      <c r="Q5" s="61"/>
+      <c r="R5" s="61"/>
+      <c r="S5" s="74"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="69"/>
-      <c r="V5" s="69"/>
+      <c r="U5" s="61"/>
+      <c r="V5" s="61"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3519,7 +3519,7 @@
       <c r="R6" s="37"/>
       <c r="S6" s="3"/>
       <c r="T6" s="40"/>
-      <c r="U6" s="61" t="s">
+      <c r="U6" s="69" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -3550,7 +3550,7 @@
       <c r="R7" s="37"/>
       <c r="S7" s="3"/>
       <c r="T7" s="40"/>
-      <c r="U7" s="62"/>
+      <c r="U7" s="70"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -3579,7 +3579,7 @@
       <c r="R8" s="37"/>
       <c r="S8" s="3"/>
       <c r="T8" s="40"/>
-      <c r="U8" s="62"/>
+      <c r="U8" s="70"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -3608,7 +3608,7 @@
       <c r="R9" s="37"/>
       <c r="S9" s="3"/>
       <c r="T9" s="40"/>
-      <c r="U9" s="62"/>
+      <c r="U9" s="70"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -3637,7 +3637,7 @@
       <c r="R10" s="37"/>
       <c r="S10" s="3"/>
       <c r="T10" s="40"/>
-      <c r="U10" s="62"/>
+      <c r="U10" s="70"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -3666,7 +3666,7 @@
       <c r="R11" s="37"/>
       <c r="S11" s="3"/>
       <c r="T11" s="40"/>
-      <c r="U11" s="62"/>
+      <c r="U11" s="70"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -3695,7 +3695,7 @@
       <c r="R12" s="37"/>
       <c r="S12" s="3"/>
       <c r="T12" s="40"/>
-      <c r="U12" s="61" t="s">
+      <c r="U12" s="69" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -3726,7 +3726,7 @@
       <c r="R13" s="9"/>
       <c r="S13" s="3"/>
       <c r="T13" s="40"/>
-      <c r="U13" s="62"/>
+      <c r="U13" s="70"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -3755,7 +3755,7 @@
       <c r="R14" s="37"/>
       <c r="S14" s="3"/>
       <c r="T14" s="40"/>
-      <c r="U14" s="62"/>
+      <c r="U14" s="70"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -3784,7 +3784,7 @@
       <c r="R15" s="37"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="62"/>
+      <c r="U15" s="70"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -3813,7 +3813,7 @@
       <c r="R16" s="37"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="63"/>
+      <c r="U16" s="71"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -5044,13 +5044,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -5062,6 +5055,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>